<commit_message>
edit TC excel file
</commit_message>
<xml_diff>
--- a/Collection of test cases.xlsx
+++ b/Collection of test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\QA_Automation_Challenge_Phuc_Le\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26541BA4-7DE8-464E-A165-65D15C4FD56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A7951B-E00E-481C-9C42-EB847F9380C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C70362BA-F476-49C5-B4CF-B98B04AFEDD7}"/>
   </bookViews>
@@ -639,8 +639,8 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>